<commit_message>
Before redoing 5 vehicle instances
</commit_message>
<xml_diff>
--- a/4 2/ExactModelData.xlsx
+++ b/4 2/ExactModelData.xlsx
@@ -1,40 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Google Drive\University\2020\Industrial Project 498\Exact Model Implementation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Google Drive\University\2020\Industrial Project 498\Exact Model Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E04DD-D766-4D17-892A-B8BC362E1A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BDB346-6ED0-41AA-93B7-7B9F7CBC9694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3615" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D" sheetId="3" r:id="rId1"/>
     <sheet name="Distances" sheetId="1" r:id="rId2"/>
     <sheet name="Times" sheetId="4" r:id="rId3"/>
-    <sheet name="HorseTrailer" sheetId="2" r:id="rId4"/>
-    <sheet name="HorseStore" sheetId="5" r:id="rId5"/>
-    <sheet name="TrailerStore" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="AverageUnload">'1D'!$L$2:$L$7</definedName>
+    <definedName name="CoordinatesX">'1D'!$G$3:$G$6</definedName>
+    <definedName name="CoordinatesY">'1D'!$H$3:$H$6</definedName>
     <definedName name="Demand">'1D'!$I$2:$I$7</definedName>
-    <definedName name="DistanceCost">'1D'!$B$2:$B$3</definedName>
+    <definedName name="DistanceCost">'1D'!$C$2:$C$3</definedName>
     <definedName name="Distances">Distances!$A$1:$F$6</definedName>
-    <definedName name="Horses">'1D'!$A$2:$A$3</definedName>
-    <definedName name="HorseStore">HorseStore!$A$1:$D$2</definedName>
-    <definedName name="HorseTrailer">HorseTrailer!$A$1:$B$2</definedName>
     <definedName name="Locations">'1D'!$F$2:$F$7</definedName>
     <definedName name="PalletCapacity">'1D'!$E$2:$E$3</definedName>
     <definedName name="Stores">'1D'!$F$3:$F$6</definedName>
-    <definedName name="TimeCost">'1D'!$C$2:$C$3</definedName>
+    <definedName name="TimeCost">'1D'!$D$2:$D$3</definedName>
     <definedName name="Times">Times!$A$1:$F$6</definedName>
-    <definedName name="Trailers">'1D'!$D$2:$D$3</definedName>
-    <definedName name="TrailerStore">TrailerStore!$A$1:$D$2</definedName>
+    <definedName name="Vehicles">'1D'!$A$2:$A$3</definedName>
+    <definedName name="VehicleTypes">'1D'!$B$2:$B$3</definedName>
     <definedName name="WindowEnd">'1D'!$K$2:$K$7</definedName>
     <definedName name="WindowStart">'1D'!$J$2:$J$7</definedName>
   </definedNames>
@@ -56,7 +52,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -78,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Pallets</t>
   </si>
@@ -98,12 +94,6 @@
     <t>Time Cost</t>
   </si>
   <si>
-    <t>Trailer</t>
-  </si>
-  <si>
-    <t>Horse</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -113,12 +103,6 @@
     <t>SP2</t>
   </si>
   <si>
-    <t>C 1</t>
-  </si>
-  <si>
-    <t>C 2</t>
-  </si>
-  <si>
     <t>Depot</t>
   </si>
   <si>
@@ -143,12 +127,6 @@
     <t>Num stores</t>
   </si>
   <si>
-    <t>Max Trailer Capacity</t>
-  </si>
-  <si>
-    <t>Min Trailer Capacity</t>
-  </si>
-  <si>
     <t>Number of vehicles</t>
   </si>
   <si>
@@ -179,10 +157,28 @@
     <t>Unload Max</t>
   </si>
   <si>
-    <t>Compatability Chance</t>
-  </si>
-  <si>
     <t>Total Demand</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Vehicle Types</t>
+  </si>
+  <si>
+    <t>Rigid</t>
+  </si>
+  <si>
+    <t>8 metre</t>
+  </si>
+  <si>
+    <t>11 metre</t>
+  </si>
+  <si>
+    <t>Number of vehicle types</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
   </si>
 </sst>
 </file>
@@ -252,17 +248,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,24 +391,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1D'!$G$2:$G$8</c:f>
+              <c:f>'1D'!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-68.589284001108666</c:v>
+                  <c:v>23.884002326657722</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-66.636522852924898</c:v>
+                  <c:v>29.495061132912241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.591685921460524</c:v>
+                  <c:v>20.898877539136237</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.010540561651766</c:v>
+                  <c:v>46.60838891126086</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -421,24 +418,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1D'!$H$2:$H$8</c:f>
+              <c:f>'1D'!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.237478643058978</c:v>
+                  <c:v>-68.159488677181429</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-75.890847876682315</c:v>
+                  <c:v>-44.906115211398074</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-20.416765050513291</c:v>
+                  <c:v>-43.948791611059448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-82.158981166325347</c:v>
+                  <c:v>-56.60345661944605</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1204,13 +1201,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1505,18 +1502,18 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.85546875" customWidth="1"/>
@@ -1536,30 +1533,30 @@
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -1571,34 +1568,46 @@
         <v>3</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="3"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">OFFSET($R$1,RANDBETWEEN(1,$P$8),0)</f>
+        <v>Rigid</v>
+      </c>
+      <c r="C2" cm="1">
+        <f t="array" aca="1" ref="C2:E2" ca="1">_xlfn.XLOOKUP(B2,OFFSET($R$2,0,0,$P$8,1),OFFSET($S$2,0,0,$P$8,3))</f>
+        <v>1.3713855068994052</v>
+      </c>
+      <c r="D2" s="8">
+        <f ca="1"/>
+        <v>14.757960314176955</v>
+      </c>
+      <c r="E2" s="2">
+        <f ca="1"/>
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" cm="1">
-        <f t="array" aca="1" ref="B2:B3" ca="1">_xlfn.RANDARRAY(P8,1,P10,P9,FALSE)</f>
-        <v>0.83626847063118803</v>
-      </c>
-      <c r="C2" s="2" cm="1">
-        <f t="array" aca="1" ref="C2:C3" ca="1">_xlfn.RANDARRAY(P8,1,P12,P11,FALSE)</f>
-        <v>12.268351655606208</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" cm="1">
-        <f t="array" aca="1" ref="E2:E3" ca="1">_xlfn.RANDARRAY(P8,1,P14,P13,TRUE)</f>
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1617,121 +1626,161 @@
       </c>
       <c r="L2" cm="1">
         <f t="array" aca="1" ref="L2:L6" ca="1">_xlfn.RANDARRAY(P2+1,1,P7,P6,FALSE)</f>
-        <v>8.122102570638029E-2</v>
+        <v>0.14362496545506762</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P2">
         <v>4</v>
       </c>
-      <c r="R2" s="7"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" cm="1">
+        <f t="array" aca="1" ref="S2:S4" ca="1">_xlfn.RANDARRAY(P8,1,P11,P10,FALSE)</f>
+        <v>1.3713855068994052</v>
+      </c>
+      <c r="T2" cm="1">
+        <f t="array" aca="1" ref="T2:T4" ca="1">_xlfn.RANDARRAY(P8,1,P13,P12,FALSE)</f>
+        <v>14.757960314176955</v>
+      </c>
+      <c r="U2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="str">
+        <f ca="1">OFFSET($R$1,RANDBETWEEN(1,$P$8),0)</f>
+        <v>8 metre</v>
+      </c>
+      <c r="C3" cm="1">
+        <f t="array" aca="1" ref="C3:E3" ca="1">_xlfn.XLOOKUP(B3,OFFSET($R$2,0,0,$P$8,1),OFFSET($S$2,0,0,$P$8,3))</f>
+        <v>1.1125014302476617</v>
+      </c>
+      <c r="D3" s="8">
         <f ca="1"/>
-        <v>0.71577426944365174</v>
-      </c>
-      <c r="C3" s="2">
-        <f ca="1"/>
-        <v>10.464096399216533</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>13.367952913375378</v>
       </c>
       <c r="E3" s="2">
         <f ca="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" cm="1">
         <f t="array" aca="1" ref="G3:H6" ca="1">_xlfn.RANDARRAY(P2,2,P4,P3,FALSE)</f>
-        <v>-68.589284001108666</v>
+        <v>23.884002326657722</v>
       </c>
       <c r="H3">
         <f ca="1"/>
-        <v>69.237478643058978</v>
+        <v>-68.159488677181429</v>
       </c>
       <c r="I3" cm="1">
-        <f t="array" aca="1" ref="I3:I6" ca="1">_xlfn.RANDARRAY(P2,1,0,ROUNDUP((P17/P2),0),TRUE)</f>
-        <v>10</v>
+        <f t="array" aca="1" ref="I3:I6" ca="1">_xlfn.RANDARRAY(P2,1,1,ROUNDUP((P15/P2),0),TRUE)</f>
+        <v>6</v>
       </c>
       <c r="J3">
         <f ca="1">IF(RAND()&lt;$P$5,RANDBETWEEN(5,23), 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K3">
         <f ca="1">IF(J3=0,24,J3+1)</f>
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="L3">
         <f ca="1"/>
-        <v>7.0393182417336608E-2</v>
+        <v>0.16009097622855867</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="P3">
         <v>100</v>
       </c>
-      <c r="R3" s="7"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3">
+        <f ca="1"/>
+        <v>1.1125014302476617</v>
+      </c>
+      <c r="T3">
+        <f ca="1"/>
+        <v>13.367952913375378</v>
+      </c>
+      <c r="U3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
         <f ca="1"/>
-        <v>-66.636522852924898</v>
+        <v>29.495061132912241</v>
       </c>
       <c r="H4">
         <f ca="1"/>
-        <v>-75.890847876682315</v>
+        <v>-44.906115211398074</v>
       </c>
       <c r="I4">
         <f ca="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J6" ca="1" si="0">IF(RAND()&lt;$P$5,RANDBETWEEN(5,23), 0)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K6" ca="1" si="1">IF(J4=0,24,J4+1)</f>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L4">
         <f ca="1"/>
-        <v>7.9235558079375712E-2</v>
+        <v>0.11739364130516822</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P4">
         <v>-100</v>
       </c>
-      <c r="R4" s="7"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4">
+        <f ca="1"/>
+        <v>1.4600515406854966</v>
+      </c>
+      <c r="T4">
+        <f ca="1"/>
+        <v>8.4843426911462956</v>
+      </c>
+      <c r="U4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5">
         <f ca="1"/>
-        <v>55.591685921460524</v>
+        <v>20.898877539136237</v>
       </c>
       <c r="H5">
         <f ca="1"/>
-        <v>-20.416765050513291</v>
+        <v>-43.948791611059448</v>
       </c>
       <c r="I5">
         <f ca="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
@@ -1743,27 +1792,27 @@
       </c>
       <c r="L5">
         <f ca="1"/>
-        <v>6.1022661362601233E-2</v>
+        <v>2.149456200733349E-2</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="P5" s="5">
         <v>0.33</v>
       </c>
-      <c r="R5" s="7"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>4</v>
       </c>
       <c r="G6">
         <f ca="1"/>
-        <v>46.010540561651766</v>
+        <v>46.60838891126086</v>
       </c>
       <c r="H6">
         <f ca="1"/>
-        <v>-82.158981166325347</v>
+        <v>-56.60345661944605</v>
       </c>
       <c r="I6">
         <f ca="1"/>
@@ -1771,28 +1820,28 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <f ca="1"/>
-        <v>0.10641561753462475</v>
+        <v>0.16490870939075775</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P6">
         <f>10/60</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1813,99 +1862,83 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="P7">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O9" s="1" t="s">
+      <c r="P13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15">
+        <f ca="1">SUM(E:E)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11">
+      <c r="P16">
+        <f ca="1">SUM(I:I)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="6">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17">
-        <f ca="1">SUM(E:E)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P18">
-        <f ca="1">SUM(I:I)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="P19" s="5">
-        <f ca="1">P18/P17</f>
-        <v>0.5957446808510638</v>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P17" s="5">
+        <f ca="1">P16/P15</f>
+        <v>0.39473684210526316</v>
       </c>
     </row>
   </sheetData>
@@ -1935,19 +1968,19 @@
       </c>
       <c r="B1">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G2)^2+('1D'!$H$3-'1D'!$H2)^2)</f>
-        <v>97.459316274190996</v>
+        <v>72.222998164536307</v>
       </c>
       <c r="C1">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G2)^2+('1D'!$H$4-'1D'!$H2)^2)</f>
-        <v>100.99429176626825</v>
+        <v>53.726323293275783</v>
       </c>
       <c r="D1">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G2)^2+('1D'!$H$5-'1D'!$H2)^2)</f>
-        <v>59.222291738146822</v>
+        <v>48.664765143460237</v>
       </c>
       <c r="E1">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G2)^2+('1D'!$H$6-'1D'!$H2)^2)</f>
-        <v>94.165110465947023</v>
+        <v>73.323210637374942</v>
       </c>
       <c r="F1">
         <f>SQRT(('1D'!$G$7-'1D'!$G2)^2+('1D'!$H$7-'1D'!$H2)^2)</f>
@@ -1957,7 +1990,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G3)^2+('1D'!$H$2-'1D'!$H3)^2)</f>
-        <v>97.459316274190996</v>
+        <v>72.222998164536307</v>
       </c>
       <c r="B2">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G3)^2+('1D'!$H$3-'1D'!$H3)^2)</f>
@@ -1965,29 +1998,29 @@
       </c>
       <c r="C2">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G3)^2+('1D'!$H$4-'1D'!$H3)^2)</f>
-        <v>145.14146352618366</v>
+        <v>23.920772530719901</v>
       </c>
       <c r="D2">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G3)^2+('1D'!$H$5-'1D'!$H3)^2)</f>
-        <v>153.16264787204639</v>
+        <v>24.394032516675111</v>
       </c>
       <c r="E2">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G3)^2+('1D'!$H$6-'1D'!$H3)^2)</f>
-        <v>189.87892940668797</v>
+        <v>25.493913441562849</v>
       </c>
       <c r="F2">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G3)^2+('1D'!$H$7-'1D'!$H3)^2)</f>
-        <v>97.459316274190996</v>
+        <v>72.222998164536307</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G4)^2+('1D'!$H$2-'1D'!$H4)^2)</f>
-        <v>100.99429176626825</v>
+        <v>53.726323293275783</v>
       </c>
       <c r="B3">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G4)^2+('1D'!$H$3-'1D'!$H4)^2)</f>
-        <v>145.14146352618366</v>
+        <v>23.920772530719901</v>
       </c>
       <c r="C3">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G4)^2+('1D'!$H$4-'1D'!$H4)^2)</f>
@@ -1995,29 +2028,29 @@
       </c>
       <c r="D3">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G4)^2+('1D'!$H$5-'1D'!$H4)^2)</f>
-        <v>134.22782455809752</v>
+        <v>8.6493260346496967</v>
       </c>
       <c r="E3">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G4)^2+('1D'!$H$6-'1D'!$H4)^2)</f>
-        <v>112.82132063960424</v>
+        <v>20.729056506885023</v>
       </c>
       <c r="F3">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G4)^2+('1D'!$H$7-'1D'!$H4)^2)</f>
-        <v>100.99429176626825</v>
+        <v>53.726323293275783</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G5)^2+('1D'!$H$2-'1D'!$H5)^2)</f>
-        <v>59.222291738146822</v>
+        <v>48.664765143460237</v>
       </c>
       <c r="B4">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G5)^2+('1D'!$H$3-'1D'!$H5)^2)</f>
-        <v>153.16264787204639</v>
+        <v>24.394032516675111</v>
       </c>
       <c r="C4">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G5)^2+('1D'!$H$4-'1D'!$H5)^2)</f>
-        <v>134.22782455809752</v>
+        <v>8.6493260346496967</v>
       </c>
       <c r="D4">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G5)^2+('1D'!$H$5-'1D'!$H5)^2)</f>
@@ -2025,29 +2058,29 @@
       </c>
       <c r="E4">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G5)^2+('1D'!$H$6-'1D'!$H5)^2)</f>
-        <v>62.481193949038989</v>
+        <v>28.655183151881783</v>
       </c>
       <c r="F4">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G5)^2+('1D'!$H$7-'1D'!$H5)^2)</f>
-        <v>59.222291738146822</v>
+        <v>48.664765143460237</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f ca="1">SQRT(('1D'!$G$2-'1D'!$G6)^2+('1D'!$H$2-'1D'!$H6)^2)</f>
-        <v>94.165110465947023</v>
+        <v>73.323210637374942</v>
       </c>
       <c r="B5">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G6)^2+('1D'!$H$3-'1D'!$H6)^2)</f>
-        <v>189.87892940668797</v>
+        <v>25.493913441562849</v>
       </c>
       <c r="C5">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G6)^2+('1D'!$H$4-'1D'!$H6)^2)</f>
-        <v>112.82132063960424</v>
+        <v>20.729056506885023</v>
       </c>
       <c r="D5">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G6)^2+('1D'!$H$5-'1D'!$H6)^2)</f>
-        <v>62.481193949038989</v>
+        <v>28.655183151881783</v>
       </c>
       <c r="E5">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G6)^2+('1D'!$H$6-'1D'!$H6)^2)</f>
@@ -2055,7 +2088,7 @@
       </c>
       <c r="F5">
         <f ca="1">SQRT(('1D'!$G$7-'1D'!$G6)^2+('1D'!$H$7-'1D'!$H6)^2)</f>
-        <v>94.165110465947023</v>
+        <v>73.323210637374942</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2065,19 +2098,19 @@
       </c>
       <c r="B6">
         <f ca="1">SQRT(('1D'!$G$3-'1D'!$G7)^2+('1D'!$H$3-'1D'!$H7)^2)</f>
-        <v>97.459316274190996</v>
+        <v>72.222998164536307</v>
       </c>
       <c r="C6">
         <f ca="1">SQRT(('1D'!$G$4-'1D'!$G7)^2+('1D'!$H$4-'1D'!$H7)^2)</f>
-        <v>100.99429176626825</v>
+        <v>53.726323293275783</v>
       </c>
       <c r="D6">
         <f ca="1">SQRT(('1D'!$G$5-'1D'!$G7)^2+('1D'!$H$5-'1D'!$H7)^2)</f>
-        <v>59.222291738146822</v>
+        <v>48.664765143460237</v>
       </c>
       <c r="E6">
         <f ca="1">SQRT(('1D'!$G$6-'1D'!$G7)^2+('1D'!$H$6-'1D'!$H7)^2)</f>
-        <v>94.165110465947023</v>
+        <v>73.323210637374942</v>
       </c>
       <c r="F6">
         <f>SQRT(('1D'!$G$7-'1D'!$G7)^2+('1D'!$H$7-'1D'!$H7)^2)</f>
@@ -2109,19 +2142,19 @@
       </c>
       <c r="B1">
         <f ca="1">Distances!B1/80</f>
-        <v>1.2182414534273875</v>
+        <v>0.90278747705670381</v>
       </c>
       <c r="C1">
         <f ca="1">Distances!C1/80</f>
-        <v>1.262428647078353</v>
+        <v>0.67157904116594724</v>
       </c>
       <c r="D1">
         <f ca="1">Distances!D1/80</f>
-        <v>0.7402786467268353</v>
+        <v>0.608309564293253</v>
       </c>
       <c r="E1">
         <f ca="1">Distances!E1/80</f>
-        <v>1.1770638808243379</v>
+        <v>0.91654013296718673</v>
       </c>
       <c r="F1">
         <f>Distances!F1/80</f>
@@ -2135,7 +2168,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">Distances!A2/80</f>
-        <v>1.2182414534273875</v>
+        <v>0.90278747705670381</v>
       </c>
       <c r="B2">
         <f ca="1">Distances!B2/80</f>
@@ -2143,19 +2176,19 @@
       </c>
       <c r="C2">
         <f ca="1">Distances!C2/80</f>
-        <v>1.8142682940772956</v>
+        <v>0.29900965663399875</v>
       </c>
       <c r="D2">
         <f ca="1">Distances!D2/80</f>
-        <v>1.9145330984005799</v>
+        <v>0.30492540645843891</v>
       </c>
       <c r="E2">
         <f ca="1">Distances!E2/80</f>
-        <v>2.3734866175835996</v>
+        <v>0.3186739180195356</v>
       </c>
       <c r="F2">
         <f ca="1">Distances!F2/80</f>
-        <v>1.2182414534273875</v>
+        <v>0.90278747705670381</v>
       </c>
       <c r="G2">
         <f>Distances!G2/80</f>
@@ -2165,11 +2198,11 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">Distances!A3/80</f>
-        <v>1.262428647078353</v>
+        <v>0.67157904116594724</v>
       </c>
       <c r="B3">
         <f ca="1">Distances!B3/80</f>
-        <v>1.8142682940772956</v>
+        <v>0.29900965663399875</v>
       </c>
       <c r="C3">
         <f ca="1">Distances!C3/80</f>
@@ -2177,15 +2210,15 @@
       </c>
       <c r="D3">
         <f ca="1">Distances!D3/80</f>
-        <v>1.677847806976219</v>
+        <v>0.10811657543312121</v>
       </c>
       <c r="E3">
         <f ca="1">Distances!E3/80</f>
-        <v>1.4102665079950529</v>
+        <v>0.25911320633606277</v>
       </c>
       <c r="F3">
         <f ca="1">Distances!F3/80</f>
-        <v>1.262428647078353</v>
+        <v>0.67157904116594724</v>
       </c>
       <c r="G3">
         <f>Distances!G3/80</f>
@@ -2195,15 +2228,15 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f ca="1">Distances!A4/80</f>
-        <v>0.7402786467268353</v>
+        <v>0.608309564293253</v>
       </c>
       <c r="B4">
         <f ca="1">Distances!B4/80</f>
-        <v>1.9145330984005799</v>
+        <v>0.30492540645843891</v>
       </c>
       <c r="C4">
         <f ca="1">Distances!C4/80</f>
-        <v>1.677847806976219</v>
+        <v>0.10811657543312121</v>
       </c>
       <c r="D4">
         <f ca="1">Distances!D4/80</f>
@@ -2211,11 +2244,11 @@
       </c>
       <c r="E4">
         <f ca="1">Distances!E4/80</f>
-        <v>0.78101492436298736</v>
+        <v>0.35818978939852231</v>
       </c>
       <c r="F4">
         <f ca="1">Distances!F4/80</f>
-        <v>0.7402786467268353</v>
+        <v>0.608309564293253</v>
       </c>
       <c r="G4">
         <f>Distances!G4/80</f>
@@ -2225,19 +2258,19 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f ca="1">Distances!A5/80</f>
-        <v>1.1770638808243379</v>
+        <v>0.91654013296718673</v>
       </c>
       <c r="B5">
         <f ca="1">Distances!B5/80</f>
-        <v>2.3734866175835996</v>
+        <v>0.3186739180195356</v>
       </c>
       <c r="C5">
         <f ca="1">Distances!C5/80</f>
-        <v>1.4102665079950529</v>
+        <v>0.25911320633606277</v>
       </c>
       <c r="D5">
         <f ca="1">Distances!D5/80</f>
-        <v>0.78101492436298736</v>
+        <v>0.35818978939852231</v>
       </c>
       <c r="E5">
         <f ca="1">Distances!E5/80</f>
@@ -2245,7 +2278,7 @@
       </c>
       <c r="F5">
         <f ca="1">Distances!F5/80</f>
-        <v>1.1770638808243379</v>
+        <v>0.91654013296718673</v>
       </c>
       <c r="G5">
         <f>Distances!G5/80</f>
@@ -2259,19 +2292,19 @@
       </c>
       <c r="B6">
         <f ca="1">Distances!B6/80</f>
-        <v>1.2182414534273875</v>
+        <v>0.90278747705670381</v>
       </c>
       <c r="C6">
         <f ca="1">Distances!C6/80</f>
-        <v>1.262428647078353</v>
+        <v>0.67157904116594724</v>
       </c>
       <c r="D6">
         <f ca="1">Distances!D6/80</f>
-        <v>0.7402786467268353</v>
+        <v>0.608309564293253</v>
       </c>
       <c r="E6">
         <f ca="1">Distances!E6/80</f>
-        <v>1.1770638808243379</v>
+        <v>0.91654013296718673</v>
       </c>
       <c r="F6">
         <f>Distances!F6/80</f>
@@ -2310,390 +2343,6 @@
       <c r="G7">
         <f>Distances!G7/80</f>
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2D636C-B1F2-40ED-AFFD-CEAECA9A3EA3}">
-  <sheetPr>
-    <tabColor theme="8"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3193DF46-A5F5-411E-9E65-0CD84739E551}">
-  <sheetPr>
-    <tabColor theme="8"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A14196F-B2E4-4597-BD06-5E39E2E8AD11}">
-  <sheetPr>
-    <tabColor theme="8"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f ca="1">IF(RAND()&lt;'1D'!$P$15,1,0)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>